<commit_message>
Documentation dossier de réalisation
</commit_message>
<xml_diff>
--- a/Documentation/Glossaire.xlsx
+++ b/Documentation/Glossaire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="174">
   <si>
     <t>Unity</t>
   </si>
@@ -1181,6 +1181,45 @@
   </si>
   <si>
     <t>cifteli</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>Colaborate</t>
+  </si>
+  <si>
+    <t>Mesh</t>
+  </si>
+  <si>
+    <t>SVG</t>
+  </si>
+  <si>
+    <t>ANSI</t>
+  </si>
+  <si>
+    <t>IEL</t>
+  </si>
+  <si>
+    <t>DIN</t>
+  </si>
+  <si>
+    <t>PNG</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Line Renderer</t>
+  </si>
+  <si>
+    <t>Collider</t>
   </si>
 </sst>
 </file>
@@ -1686,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,6 +2211,76 @@
       </c>
       <c r="B67" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fixes & comments & documentation
</commit_message>
<xml_diff>
--- a/Documentation/Glossaire.xlsx
+++ b/Documentation/Glossaire.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="180">
   <si>
     <t>Unity</t>
   </si>
@@ -1220,6 +1220,24 @@
   </si>
   <si>
     <t>Collider</t>
+  </si>
+  <si>
+    <t>Serializer</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Çifteli</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1725,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,6 +2299,31 @@
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2299,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,22 +2353,31 @@
     <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>

</xml_diff>